<commit_message>
Getting back to work on the project
</commit_message>
<xml_diff>
--- a/Sub-System Design and Documentation/Structural Assembly/Washing Machine Sizing Calculations.xlsx
+++ b/Sub-System Design and Documentation/Structural Assembly/Washing Machine Sizing Calculations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tommy\Documents\Repositories\Microgravity-Press-Washing-Machine\Sub-System Design and Documentation\Structural Assembly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A281FD-A3E7-4339-BCAD-1540E09B0953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C60DD5-2232-4AF1-894D-CDF8BB936C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <sheet name="Chamber and Piston Attributes" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>

</xml_diff>